<commit_message>
Refactor results module and fix DelayProcessor integration
Major changes:
- Consolidated 8 duplicate files in src/results into 6 unified modules
- Fixed DelayProcessor integration in scheduler for accurate setup time calculation
- Enhanced gap_analyzer with detailed setup condition analysis
- Removed redundant files and improved code organization
- Added comprehensive gap analysis with DelayProcessor key values
</commit_message>
<xml_diff>
--- a/python_engine/data/output/machine_gap_summary.xlsx
+++ b/python_engine/data/output/machine_gap_summary.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,11 +464,6 @@
           <t>total_theoretical_setup_time</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>setup_efficiency</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -481,16 +476,13 @@
         <v>185</v>
       </c>
       <c r="D2" t="n">
-        <v>108</v>
+        <v>126</v>
       </c>
       <c r="E2" t="n">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="F2" t="n">
         <v>126</v>
-      </c>
-      <c r="G2" t="n">
-        <v>85.7</v>
       </c>
     </row>
     <row r="3">
@@ -512,9 +504,6 @@
       <c r="F3" t="n">
         <v>0</v>
       </c>
-      <c r="G3" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -535,9 +524,6 @@
       <c r="F4" t="n">
         <v>340</v>
       </c>
-      <c r="G4" t="n">
-        <v>100</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -547,19 +533,16 @@
         <v>95</v>
       </c>
       <c r="C5" t="n">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D5" t="n">
-        <v>190</v>
+        <v>218</v>
       </c>
       <c r="E5" t="n">
-        <v>106</v>
+        <v>76</v>
       </c>
       <c r="F5" t="n">
         <v>218</v>
-      </c>
-      <c r="G5" t="n">
-        <v>87.2</v>
       </c>
     </row>
     <row r="6">
@@ -579,9 +562,6 @@
         <v>243</v>
       </c>
       <c r="F6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G6" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update local development files and fix preprocessing errors
- Modified config.py and main.py for better data handling
- Updated preprocessing module to handle empty data cases
- Added new input data file (python_input.xlsx)
- Removed old sample data files that are no longer used
- Updated output files with latest processing results
</commit_message>
<xml_diff>
--- a/python_engine/data/output/machine_gap_summary.xlsx
+++ b/python_engine/data/output/machine_gap_summary.xlsx
@@ -473,13 +473,13 @@
         <v>2</v>
       </c>
       <c r="C2" t="n">
-        <v>80</v>
+        <v>32</v>
       </c>
       <c r="D2" t="n">
         <v>4</v>
       </c>
       <c r="E2" t="n">
-        <v>76</v>
+        <v>28</v>
       </c>
       <c r="F2" t="n">
         <v>4</v>

</xml_diff>

<commit_message>
MIXTURE_LOGIC.md, machine_gap_summary.xlsx, schedule_gaps_detailed.xlsx, 생산계획 DB 기준정보 테이블 0930.xlsx 업데이트
</commit_message>
<xml_diff>
--- a/python_engine/data/output/machine_gap_summary.xlsx
+++ b/python_engine/data/output/machine_gap_summary.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -485,46 +485,6 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>3</v>
-      </c>
-      <c r="B3" t="n">
-        <v>1</v>
-      </c>
-      <c r="C3" t="n">
-        <v>4</v>
-      </c>
-      <c r="D3" t="n">
-        <v>4</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>4</v>
-      </c>
-      <c r="B4" t="n">
-        <v>5</v>
-      </c>
-      <c r="C4" t="n">
-        <v>14</v>
-      </c>
-      <c r="D4" t="n">
-        <v>8</v>
-      </c>
-      <c r="E4" t="n">
-        <v>6</v>
-      </c>
-      <c r="F4" t="n">
-        <v>8</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>